<commit_message>
mss11o gotowe okrk poprawiony excell
</commit_message>
<xml_diff>
--- a/Statystyki_2018/Template/okrk_.xlsx
+++ b/Statystyki_2018/Template/okrk_.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Czas sesyjny w okresie od 1.01.2017 do 31.12.2017 roku</t>
   </si>
@@ -164,12 +164,6 @@
   </si>
   <si>
     <t>Nowak</t>
-  </si>
-  <si>
-    <t>6023.15</t>
-  </si>
-  <si>
-    <t>8023.15</t>
   </si>
   <si>
     <t>Michał</t>
@@ -475,7 +469,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -928,13 +922,130 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="98">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="2"/>
@@ -1176,13 +1287,29 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="31" applyBorder="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="32" applyBorder="1" xfId="0">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="33" applyBorder="1" xfId="0">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="32" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="34" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="35" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="36" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="37" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="38" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="39" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="40" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="41" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="42" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="43" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="44" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="43" applyBorder="1" xfId="0">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1736,26 +1863,26 @@
         <v>20</v>
       </c>
       <c r="F6" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="49" t="s">
         <v>71</v>
-      </c>
-      <c r="G6" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>73</v>
       </c>
       <c r="I6" s="50"/>
       <c r="J6" s="36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K6" s="37"/>
       <c r="L6" s="37"/>
       <c r="M6" s="38"/>
       <c r="N6" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P6" s="21"/>
       <c r="Q6" s="21"/>
@@ -1778,22 +1905,22 @@
       <c r="F7" s="46"/>
       <c r="G7" s="25"/>
       <c r="H7" s="32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I7" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J7" s="39" t="s">
         <v>30</v>
       </c>
       <c r="K7" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7" s="55" t="s">
         <v>79</v>
-      </c>
-      <c r="L7" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="M7" s="55" t="s">
-        <v>81</v>
       </c>
       <c r="N7" s="18"/>
       <c r="O7" s="24" t="s">
@@ -1856,746 +1983,587 @@
       <c r="X8" s="14"/>
     </row>
     <row r="9">
-      <c r="A9" s="83">
+      <c r="A9" s="84">
         <v>1</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="84" t="s">
+      <c r="E9" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="85">
-        <v>0</v>
-      </c>
-      <c r="G9" s="85">
-        <v>0</v>
-      </c>
-      <c r="H9" s="85">
-        <v>0</v>
-      </c>
-      <c r="I9" s="85">
-        <v>0</v>
-      </c>
-      <c r="J9" s="85">
-        <v>0</v>
-      </c>
-      <c r="K9" s="85">
-        <v>0</v>
-      </c>
-      <c r="L9" s="85">
-        <v>0</v>
-      </c>
-      <c r="M9" s="85">
-        <v>0</v>
-      </c>
-      <c r="N9" s="85">
-        <v>0</v>
-      </c>
-      <c r="O9" s="85">
-        <v>0</v>
-      </c>
-      <c r="P9" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="85">
-        <v>0</v>
-      </c>
-      <c r="R9" s="85">
-        <v>0</v>
-      </c>
-      <c r="S9" s="85">
-        <v>0</v>
-      </c>
-      <c r="T9" s="85">
-        <v>0</v>
-      </c>
-      <c r="U9" s="85">
-        <v>0</v>
-      </c>
-      <c r="V9" s="85">
-        <v>0</v>
-      </c>
-      <c r="W9" s="85">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" s="83">
+      <c r="A10" s="84">
         <v>2</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="84" t="s">
+      <c r="E10" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="85">
-        <v>0</v>
-      </c>
-      <c r="G10" s="85">
-        <v>0</v>
-      </c>
-      <c r="H10" s="85">
-        <v>0</v>
-      </c>
-      <c r="I10" s="85">
-        <v>0</v>
-      </c>
-      <c r="J10" s="85">
-        <v>0</v>
-      </c>
-      <c r="K10" s="85">
-        <v>0</v>
-      </c>
-      <c r="L10" s="85">
-        <v>0</v>
-      </c>
-      <c r="M10" s="85">
-        <v>0</v>
-      </c>
-      <c r="N10" s="85">
-        <v>0</v>
-      </c>
-      <c r="O10" s="85">
-        <v>0</v>
-      </c>
-      <c r="P10" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="85">
-        <v>0</v>
-      </c>
-      <c r="R10" s="85">
-        <v>0</v>
-      </c>
-      <c r="S10" s="85">
-        <v>0</v>
-      </c>
-      <c r="T10" s="85">
-        <v>0</v>
-      </c>
-      <c r="U10" s="85">
-        <v>0</v>
-      </c>
-      <c r="V10" s="85">
-        <v>0</v>
-      </c>
-      <c r="W10" s="85">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
-      <c r="A11" s="83">
+      <c r="A11" s="84">
         <v>3</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="84" t="s">
+      <c r="E11" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="85">
-        <v>0</v>
-      </c>
-      <c r="G11" s="85">
-        <v>0</v>
-      </c>
-      <c r="H11" s="85">
-        <v>0</v>
-      </c>
-      <c r="I11" s="85">
-        <v>0</v>
-      </c>
-      <c r="J11" s="85">
-        <v>0</v>
-      </c>
-      <c r="K11" s="85">
-        <v>0</v>
-      </c>
-      <c r="L11" s="85">
-        <v>0</v>
-      </c>
-      <c r="M11" s="85">
-        <v>0</v>
-      </c>
-      <c r="N11" s="85">
-        <v>0</v>
-      </c>
-      <c r="O11" s="85">
-        <v>0</v>
-      </c>
-      <c r="P11" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="85">
-        <v>0</v>
-      </c>
-      <c r="R11" s="85">
-        <v>0</v>
-      </c>
-      <c r="S11" s="85">
-        <v>0</v>
-      </c>
-      <c r="T11" s="85">
-        <v>0</v>
-      </c>
-      <c r="U11" s="85">
-        <v>0</v>
-      </c>
-      <c r="V11" s="85">
-        <v>0</v>
-      </c>
-      <c r="W11" s="85">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
-      <c r="A12" s="83">
+      <c r="A12" s="84">
         <v>4</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="84" t="s">
+      <c r="D12" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="84" t="s">
+      <c r="E12" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="85">
-        <v>2038</v>
-      </c>
-      <c r="G12" s="85">
-        <v>0</v>
-      </c>
-      <c r="H12" s="85">
-        <v>0</v>
-      </c>
-      <c r="I12" s="85">
-        <v>0</v>
-      </c>
-      <c r="J12" s="85">
-        <v>0</v>
-      </c>
-      <c r="K12" s="85" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" s="84">
+        <v>5</v>
+      </c>
+      <c r="B13" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="85">
-        <v>0</v>
-      </c>
-      <c r="M12" s="85" t="s">
+      <c r="E13" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="N12" s="85">
-        <v>0</v>
-      </c>
-      <c r="O12" s="85">
-        <v>0</v>
-      </c>
-      <c r="P12" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="85">
-        <v>0</v>
-      </c>
-      <c r="R12" s="85">
-        <v>0</v>
-      </c>
-      <c r="S12" s="85">
-        <v>0</v>
-      </c>
-      <c r="T12" s="85">
-        <v>0</v>
-      </c>
-      <c r="U12" s="85">
-        <v>0</v>
-      </c>
-      <c r="V12" s="85">
-        <v>0</v>
-      </c>
-      <c r="W12" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="83">
-        <v>5</v>
-      </c>
-      <c r="B13" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="84" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" s="84">
+        <v>6</v>
+      </c>
+      <c r="B14" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="C14" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="85">
-        <v>2056</v>
-      </c>
-      <c r="G13" s="85">
-        <v>0</v>
-      </c>
-      <c r="H13" s="85">
-        <v>0</v>
-      </c>
-      <c r="I13" s="85">
-        <v>0</v>
-      </c>
-      <c r="J13" s="85">
-        <v>0</v>
-      </c>
-      <c r="K13" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="L13" s="85">
-        <v>0</v>
-      </c>
-      <c r="M13" s="85" t="s">
+      <c r="D14" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="85" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="86"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="96"/>
+      <c r="O15" s="84">
+        <v>11</v>
+      </c>
+      <c r="P15" s="83"/>
+      <c r="Q15" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="R15" s="84">
+        <v>0</v>
+      </c>
+      <c r="S15" s="84">
+        <v>41</v>
+      </c>
+      <c r="T15" s="97">
+        <v>0</v>
+      </c>
+      <c r="U15" s="96"/>
+      <c r="V15" s="84">
+        <v>61</v>
+      </c>
+      <c r="W15" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="89"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="95" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="94"/>
+      <c r="N16" s="96"/>
+      <c r="O16" s="84">
+        <v>0</v>
+      </c>
+      <c r="P16" s="83"/>
+      <c r="Q16" s="84">
+        <v>0</v>
+      </c>
+      <c r="R16" s="84">
+        <v>0</v>
+      </c>
+      <c r="S16" s="84">
+        <v>42</v>
+      </c>
+      <c r="T16" s="97">
+        <v>52</v>
+      </c>
+      <c r="U16" s="96"/>
+      <c r="V16" s="84">
+        <v>62</v>
+      </c>
+      <c r="W16" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="89"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="94"/>
+      <c r="K17" s="94"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="94"/>
+      <c r="N17" s="96"/>
+      <c r="O17" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="84">
+        <v>0</v>
+      </c>
+      <c r="R17" s="84">
+        <v>33</v>
+      </c>
+      <c r="S17" s="84">
+        <v>0</v>
+      </c>
+      <c r="T17" s="97">
+        <v>0</v>
+      </c>
+      <c r="U17" s="96"/>
+      <c r="V17" s="84">
+        <v>0</v>
+      </c>
+      <c r="W17" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="89"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="95" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="94"/>
+      <c r="N18" s="96"/>
+      <c r="O18" s="84">
+        <v>0</v>
+      </c>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="84">
+        <v>0</v>
+      </c>
+      <c r="R18" s="84">
+        <v>0</v>
+      </c>
+      <c r="S18" s="84">
+        <v>0</v>
+      </c>
+      <c r="T18" s="97">
+        <v>0</v>
+      </c>
+      <c r="U18" s="96"/>
+      <c r="V18" s="84">
+        <v>0</v>
+      </c>
+      <c r="W18" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="89"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="94"/>
+      <c r="L19" s="94"/>
+      <c r="M19" s="94"/>
+      <c r="N19" s="96"/>
+      <c r="O19" s="84">
+        <v>0</v>
+      </c>
+      <c r="P19" s="83"/>
+      <c r="Q19" s="84">
+        <v>0</v>
+      </c>
+      <c r="R19" s="84">
+        <v>0</v>
+      </c>
+      <c r="S19" s="84">
+        <v>0</v>
+      </c>
+      <c r="T19" s="97">
+        <v>55</v>
+      </c>
+      <c r="U19" s="96"/>
+      <c r="V19" s="84">
+        <v>0</v>
+      </c>
+      <c r="W19" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="89"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="95" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="94"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="94"/>
+      <c r="M20" s="94"/>
+      <c r="N20" s="96"/>
+      <c r="O20" s="84">
+        <v>0</v>
+      </c>
+      <c r="P20" s="83"/>
+      <c r="Q20" s="84">
+        <v>3</v>
+      </c>
+      <c r="R20" s="84">
+        <v>0</v>
+      </c>
+      <c r="S20" s="84">
+        <v>0</v>
+      </c>
+      <c r="T20" s="97">
+        <v>0</v>
+      </c>
+      <c r="U20" s="96"/>
+      <c r="V20" s="84">
+        <v>66</v>
+      </c>
+      <c r="W20" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="89"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="94"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="94"/>
+      <c r="J21" s="94"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="94"/>
+      <c r="M21" s="94"/>
+      <c r="N21" s="96"/>
+      <c r="O21" s="84">
+        <v>0</v>
+      </c>
+      <c r="P21" s="83"/>
+      <c r="Q21" s="84">
+        <v>0</v>
+      </c>
+      <c r="R21" s="84">
+        <v>0</v>
+      </c>
+      <c r="S21" s="84">
+        <v>0</v>
+      </c>
+      <c r="T21" s="97">
+        <v>0</v>
+      </c>
+      <c r="U21" s="96"/>
+      <c r="V21" s="84">
+        <v>67</v>
+      </c>
+      <c r="W21" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="89"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="86"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="94"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="96"/>
+      <c r="O22" s="84">
+        <v>81</v>
+      </c>
+      <c r="P22" s="83"/>
+      <c r="Q22" s="84">
+        <v>0</v>
+      </c>
+      <c r="R22" s="84">
+        <v>0</v>
+      </c>
+      <c r="S22" s="84">
         <v>48</v>
       </c>
-      <c r="N13" s="85">
-        <v>0</v>
-      </c>
-      <c r="O13" s="85">
-        <v>0</v>
-      </c>
-      <c r="P13" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="85">
-        <v>0</v>
-      </c>
-      <c r="R13" s="85">
-        <v>0</v>
-      </c>
-      <c r="S13" s="85">
-        <v>0</v>
-      </c>
-      <c r="T13" s="85">
-        <v>0</v>
-      </c>
-      <c r="U13" s="85">
-        <v>0</v>
-      </c>
-      <c r="V13" s="85">
-        <v>0</v>
-      </c>
-      <c r="W13" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="83">
-        <v>6</v>
-      </c>
-      <c r="B14" s="83" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="84" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="84" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="85">
-        <v>0</v>
-      </c>
-      <c r="G14" s="85">
-        <v>0</v>
-      </c>
-      <c r="H14" s="85">
-        <v>0</v>
-      </c>
-      <c r="I14" s="85">
-        <v>0</v>
-      </c>
-      <c r="J14" s="85">
-        <v>0</v>
-      </c>
-      <c r="K14" s="85">
-        <v>0</v>
-      </c>
-      <c r="L14" s="85">
-        <v>0</v>
-      </c>
-      <c r="M14" s="85">
-        <v>0</v>
-      </c>
-      <c r="N14" s="85">
-        <v>0</v>
-      </c>
-      <c r="O14" s="85">
-        <v>0</v>
-      </c>
-      <c r="P14" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="85">
-        <v>0</v>
-      </c>
-      <c r="R14" s="85">
-        <v>0</v>
-      </c>
-      <c r="S14" s="85">
-        <v>0</v>
-      </c>
-      <c r="T14" s="85">
-        <v>0</v>
-      </c>
-      <c r="U14" s="85">
-        <v>0</v>
-      </c>
-      <c r="V14" s="85">
-        <v>0</v>
-      </c>
-      <c r="W14" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="85" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="O15" s="83">
-        <v>11</v>
-      </c>
-      <c r="Q15" s="83" t="s">
-        <v>83</v>
-      </c>
-      <c r="R15" s="83">
-        <v>0</v>
-      </c>
-      <c r="S15" s="83">
-        <v>41</v>
-      </c>
-      <c r="T15" s="83">
-        <v>51</v>
-      </c>
-      <c r="V15" s="83">
-        <v>61</v>
-      </c>
-      <c r="W15" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="D16" s="85" t="s">
-        <v>84</v>
-      </c>
-      <c r="O16" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="83">
-        <v>0</v>
-      </c>
-      <c r="R16" s="83">
-        <v>0</v>
-      </c>
-      <c r="S16" s="83">
-        <v>42</v>
-      </c>
-      <c r="T16" s="83">
-        <v>52</v>
-      </c>
-      <c r="V16" s="83">
-        <v>62</v>
-      </c>
-      <c r="W16" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="D17" s="85" t="s">
-        <v>85</v>
-      </c>
-      <c r="O17" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="83">
-        <v>0</v>
-      </c>
-      <c r="R17" s="83">
-        <v>33</v>
-      </c>
-      <c r="S17" s="83">
-        <v>0</v>
-      </c>
-      <c r="T17" s="83">
-        <v>0</v>
-      </c>
-      <c r="V17" s="83">
-        <v>0</v>
-      </c>
-      <c r="W17" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="D18" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="O18" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="83">
-        <v>0</v>
-      </c>
-      <c r="R18" s="83">
-        <v>0</v>
-      </c>
-      <c r="S18" s="83">
-        <v>0</v>
-      </c>
-      <c r="T18" s="83">
-        <v>0</v>
-      </c>
-      <c r="V18" s="83">
-        <v>0</v>
-      </c>
-      <c r="W18" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="D19" s="85" t="s">
-        <v>87</v>
-      </c>
-      <c r="O19" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="83">
-        <v>0</v>
-      </c>
-      <c r="R19" s="83">
-        <v>0</v>
-      </c>
-      <c r="S19" s="83">
-        <v>0</v>
-      </c>
-      <c r="T19" s="83">
-        <v>55</v>
-      </c>
-      <c r="V19" s="83">
-        <v>0</v>
-      </c>
-      <c r="W19" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="D20" s="85" t="s">
-        <v>88</v>
-      </c>
-      <c r="O20" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="83">
-        <v>3</v>
-      </c>
-      <c r="R20" s="83">
-        <v>0</v>
-      </c>
-      <c r="S20" s="83">
-        <v>0</v>
-      </c>
-      <c r="T20" s="83">
-        <v>0</v>
-      </c>
-      <c r="V20" s="83">
-        <v>66</v>
-      </c>
-      <c r="W20" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="D21" s="85" t="s">
-        <v>89</v>
-      </c>
-      <c r="O21" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="83">
-        <v>0</v>
-      </c>
-      <c r="R21" s="83">
-        <v>0</v>
-      </c>
-      <c r="S21" s="83">
-        <v>0</v>
-      </c>
-      <c r="T21" s="83">
-        <v>0</v>
-      </c>
-      <c r="V21" s="83">
-        <v>67</v>
-      </c>
-      <c r="W21" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="D22" s="85" t="s">
+      <c r="T22" s="97">
+        <v>58</v>
+      </c>
+      <c r="U22" s="96"/>
+      <c r="V22" s="84">
+        <v>68</v>
+      </c>
+      <c r="W22" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="89"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="89"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="95" t="s">
         <v>90</v>
       </c>
-      <c r="G22" s="85" t="s">
+      <c r="H23" s="94"/>
+      <c r="I23" s="94"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="94"/>
+      <c r="M23" s="94"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="84">
+        <v>0</v>
+      </c>
+      <c r="P23" s="83"/>
+      <c r="Q23" s="84">
+        <v>0</v>
+      </c>
+      <c r="R23" s="84">
+        <v>0</v>
+      </c>
+      <c r="S23" s="84">
+        <v>49</v>
+      </c>
+      <c r="T23" s="97">
+        <v>59</v>
+      </c>
+      <c r="U23" s="96"/>
+      <c r="V23" s="84">
+        <v>69</v>
+      </c>
+      <c r="W23" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="89"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="89"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="95" t="s">
         <v>91</v>
       </c>
-      <c r="O22" s="83">
-        <v>81</v>
-      </c>
-      <c r="Q22" s="83">
-        <v>0</v>
-      </c>
-      <c r="R22" s="83">
-        <v>0</v>
-      </c>
-      <c r="S22" s="83">
-        <v>48</v>
-      </c>
-      <c r="T22" s="83">
-        <v>58</v>
-      </c>
-      <c r="V22" s="83">
-        <v>68</v>
-      </c>
-      <c r="W22" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="G23" s="85" t="s">
+      <c r="H24" s="94"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="94"/>
+      <c r="K24" s="94"/>
+      <c r="L24" s="94"/>
+      <c r="M24" s="94"/>
+      <c r="N24" s="96"/>
+      <c r="O24" s="84">
+        <v>0</v>
+      </c>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="84">
+        <v>0</v>
+      </c>
+      <c r="R24" s="84">
+        <v>0</v>
+      </c>
+      <c r="S24" s="84">
+        <v>0</v>
+      </c>
+      <c r="T24" s="97">
+        <v>0</v>
+      </c>
+      <c r="U24" s="96"/>
+      <c r="V24" s="84">
+        <v>0</v>
+      </c>
+      <c r="W24" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="89"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="89"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="95" t="s">
         <v>92</v>
       </c>
-      <c r="O23" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="83">
-        <v>0</v>
-      </c>
-      <c r="R23" s="83">
-        <v>0</v>
-      </c>
-      <c r="S23" s="83">
-        <v>49</v>
-      </c>
-      <c r="T23" s="83">
-        <v>59</v>
-      </c>
-      <c r="V23" s="83">
-        <v>69</v>
-      </c>
-      <c r="W23" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="G24" s="85" t="s">
+      <c r="H25" s="94"/>
+      <c r="I25" s="94"/>
+      <c r="J25" s="94"/>
+      <c r="K25" s="94"/>
+      <c r="L25" s="94"/>
+      <c r="M25" s="94"/>
+      <c r="N25" s="96"/>
+      <c r="O25" s="84">
+        <v>0</v>
+      </c>
+      <c r="P25" s="83"/>
+      <c r="Q25" s="84">
+        <v>0</v>
+      </c>
+      <c r="R25" s="84">
+        <v>0</v>
+      </c>
+      <c r="S25" s="84">
+        <v>0</v>
+      </c>
+      <c r="T25" s="97">
+        <v>0</v>
+      </c>
+      <c r="U25" s="96"/>
+      <c r="V25" s="84">
+        <v>0</v>
+      </c>
+      <c r="W25" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="90"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="95" t="s">
         <v>93</v>
       </c>
-      <c r="O24" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="83">
-        <v>0</v>
-      </c>
-      <c r="R24" s="83">
-        <v>0</v>
-      </c>
-      <c r="S24" s="83">
-        <v>0</v>
-      </c>
-      <c r="T24" s="83">
-        <v>0</v>
-      </c>
-      <c r="V24" s="83">
-        <v>0</v>
-      </c>
-      <c r="W24" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="G25" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="O25" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="83">
-        <v>0</v>
-      </c>
-      <c r="R25" s="83">
-        <v>0</v>
-      </c>
-      <c r="S25" s="83">
-        <v>0</v>
-      </c>
-      <c r="T25" s="83">
-        <v>0</v>
-      </c>
-      <c r="V25" s="83">
-        <v>0</v>
-      </c>
-      <c r="W25" s="83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="G26" s="85" t="s">
-        <v>95</v>
-      </c>
-      <c r="O26" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="83">
-        <v>0</v>
-      </c>
-      <c r="R26" s="83">
-        <v>0</v>
-      </c>
-      <c r="S26" s="83">
-        <v>0</v>
-      </c>
-      <c r="T26" s="83">
-        <v>0</v>
-      </c>
-      <c r="V26" s="83">
-        <v>0</v>
-      </c>
-      <c r="W26" s="83">
+      <c r="H26" s="94"/>
+      <c r="I26" s="94"/>
+      <c r="J26" s="94"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="94"/>
+      <c r="M26" s="94"/>
+      <c r="N26" s="96"/>
+      <c r="O26" s="84">
+        <v>0</v>
+      </c>
+      <c r="P26" s="83"/>
+      <c r="Q26" s="84">
+        <v>0</v>
+      </c>
+      <c r="R26" s="84">
+        <v>0</v>
+      </c>
+      <c r="S26" s="84">
+        <v>0</v>
+      </c>
+      <c r="T26" s="97">
+        <v>0</v>
+      </c>
+      <c r="U26" s="96"/>
+      <c r="V26" s="84">
+        <v>0</v>
+      </c>
+      <c r="W26" s="84">
         <v>0</v>
       </c>
     </row>
@@ -2987,393 +2955,105 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9">
-      <c r="A9" s="83">
+      <c r="A9" s="84">
         <v>1</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="84" t="s">
+      <c r="E9" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="85">
-        <v>0</v>
-      </c>
-      <c r="G9" s="85">
-        <v>0</v>
-      </c>
-      <c r="H9" s="85">
-        <v>0</v>
-      </c>
-      <c r="I9" s="85">
-        <v>0</v>
-      </c>
-      <c r="J9" s="85">
-        <v>0</v>
-      </c>
-      <c r="K9" s="85">
-        <v>0</v>
-      </c>
-      <c r="L9" s="85">
-        <v>0</v>
-      </c>
-      <c r="M9" s="85">
-        <v>0</v>
-      </c>
-      <c r="N9" s="85">
-        <v>0</v>
-      </c>
-      <c r="O9" s="85">
-        <v>0</v>
-      </c>
-      <c r="P9" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="85">
-        <v>0</v>
-      </c>
-      <c r="R9" s="85">
-        <v>0</v>
-      </c>
-      <c r="S9" s="85">
-        <v>0</v>
-      </c>
-      <c r="T9" s="85">
-        <v>0</v>
-      </c>
-      <c r="U9" s="85">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" s="83">
+      <c r="A10" s="84">
         <v>2</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="84" t="s">
+      <c r="E10" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="85">
-        <v>0</v>
-      </c>
-      <c r="G10" s="85">
-        <v>0</v>
-      </c>
-      <c r="H10" s="85">
-        <v>0</v>
-      </c>
-      <c r="I10" s="85">
-        <v>0</v>
-      </c>
-      <c r="J10" s="85">
-        <v>0</v>
-      </c>
-      <c r="K10" s="85">
-        <v>0</v>
-      </c>
-      <c r="L10" s="85">
-        <v>0</v>
-      </c>
-      <c r="M10" s="85">
-        <v>0</v>
-      </c>
-      <c r="N10" s="85">
-        <v>0</v>
-      </c>
-      <c r="O10" s="85">
-        <v>0</v>
-      </c>
-      <c r="P10" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="85">
-        <v>0</v>
-      </c>
-      <c r="R10" s="85">
-        <v>0</v>
-      </c>
-      <c r="S10" s="85">
-        <v>0</v>
-      </c>
-      <c r="T10" s="85">
-        <v>0</v>
-      </c>
-      <c r="U10" s="85">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
-      <c r="A11" s="83">
+      <c r="A11" s="84">
         <v>3</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="84" t="s">
+      <c r="E11" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="85">
-        <v>0</v>
-      </c>
-      <c r="G11" s="85">
-        <v>0</v>
-      </c>
-      <c r="H11" s="85">
-        <v>0</v>
-      </c>
-      <c r="I11" s="85">
-        <v>0</v>
-      </c>
-      <c r="J11" s="85">
-        <v>0</v>
-      </c>
-      <c r="K11" s="85">
-        <v>0</v>
-      </c>
-      <c r="L11" s="85">
-        <v>0</v>
-      </c>
-      <c r="M11" s="85">
-        <v>0</v>
-      </c>
-      <c r="N11" s="85">
-        <v>0</v>
-      </c>
-      <c r="O11" s="85">
-        <v>0</v>
-      </c>
-      <c r="P11" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="85">
-        <v>0</v>
-      </c>
-      <c r="R11" s="85">
-        <v>0</v>
-      </c>
-      <c r="S11" s="85">
-        <v>0</v>
-      </c>
-      <c r="T11" s="85">
-        <v>0</v>
-      </c>
-      <c r="U11" s="85">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
-      <c r="A12" s="83">
+      <c r="A12" s="84">
         <v>4</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="84" t="s">
+      <c r="D12" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="84" t="s">
+      <c r="E12" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="85">
-        <v>0</v>
-      </c>
-      <c r="G12" s="85">
-        <v>0</v>
-      </c>
-      <c r="H12" s="85">
-        <v>0</v>
-      </c>
-      <c r="I12" s="85">
-        <v>0</v>
-      </c>
-      <c r="J12" s="85">
-        <v>0</v>
-      </c>
-      <c r="K12" s="85" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" s="84">
+        <v>5</v>
+      </c>
+      <c r="B13" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="85">
-        <v>0</v>
-      </c>
-      <c r="M12" s="85" t="s">
+      <c r="E13" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="N12" s="85">
-        <v>0</v>
-      </c>
-      <c r="O12" s="85">
-        <v>0</v>
-      </c>
-      <c r="P12" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="85">
-        <v>0</v>
-      </c>
-      <c r="R12" s="85">
-        <v>0</v>
-      </c>
-      <c r="S12" s="85">
-        <v>0</v>
-      </c>
-      <c r="T12" s="85">
-        <v>0</v>
-      </c>
-      <c r="U12" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="83">
-        <v>5</v>
-      </c>
-      <c r="B13" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="84" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" s="84">
+        <v>6</v>
+      </c>
+      <c r="B14" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="C14" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="85">
-        <v>0</v>
-      </c>
-      <c r="G13" s="85">
-        <v>0</v>
-      </c>
-      <c r="H13" s="85">
-        <v>0</v>
-      </c>
-      <c r="I13" s="85">
-        <v>0</v>
-      </c>
-      <c r="J13" s="85">
-        <v>0</v>
-      </c>
-      <c r="K13" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="L13" s="85">
-        <v>0</v>
-      </c>
-      <c r="M13" s="85" t="s">
-        <v>48</v>
-      </c>
-      <c r="N13" s="85">
-        <v>0</v>
-      </c>
-      <c r="O13" s="85">
-        <v>0</v>
-      </c>
-      <c r="P13" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="85">
-        <v>0</v>
-      </c>
-      <c r="R13" s="85">
-        <v>0</v>
-      </c>
-      <c r="S13" s="85">
-        <v>0</v>
-      </c>
-      <c r="T13" s="85">
-        <v>0</v>
-      </c>
-      <c r="U13" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="83">
-        <v>6</v>
-      </c>
-      <c r="B14" s="83" t="s">
+      <c r="D14" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="E14" s="85" t="s">
         <v>52</v>
-      </c>
-      <c r="D14" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="84" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="85">
-        <v>0</v>
-      </c>
-      <c r="G14" s="85">
-        <v>0</v>
-      </c>
-      <c r="H14" s="85">
-        <v>0</v>
-      </c>
-      <c r="I14" s="85">
-        <v>0</v>
-      </c>
-      <c r="J14" s="85">
-        <v>0</v>
-      </c>
-      <c r="K14" s="85">
-        <v>0</v>
-      </c>
-      <c r="L14" s="85">
-        <v>0</v>
-      </c>
-      <c r="M14" s="85">
-        <v>0</v>
-      </c>
-      <c r="N14" s="85">
-        <v>0</v>
-      </c>
-      <c r="O14" s="85">
-        <v>0</v>
-      </c>
-      <c r="P14" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="85">
-        <v>0</v>
-      </c>
-      <c r="R14" s="85">
-        <v>0</v>
-      </c>
-      <c r="S14" s="85">
-        <v>0</v>
-      </c>
-      <c r="T14" s="85">
-        <v>0</v>
-      </c>
-      <c r="U14" s="85">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3454,10 +3134,10 @@
   <sheetData>
     <row r="1" ht="15">
       <c r="A1" s="75" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="78" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="78"/>
       <c r="D1" s="78"/>
@@ -3472,18 +3152,18 @@
     <row r="2" ht="15">
       <c r="A2" s="76"/>
       <c r="B2" s="79" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2" s="79"/>
       <c r="E2" s="80" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F2" s="80"/>
       <c r="G2" s="74" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H2" s="74"/>
       <c r="I2" s="74"/>
@@ -3494,43 +3174,43 @@
       <c r="A3" s="76"/>
       <c r="B3" s="79"/>
       <c r="C3" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" s="80"/>
       <c r="F3" s="80"/>
       <c r="G3" s="79" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="J3" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="79" t="s">
+      <c r="K3" s="74" t="s">
         <v>64</v>
-      </c>
-      <c r="J3" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" s="74" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" ht="45">
       <c r="A4" s="77"/>
       <c r="B4" s="79"/>
       <c r="C4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="G4" s="79"/>
       <c r="H4" s="79"/>

</xml_diff>